<commit_message>
Update RuleSet mapping Transport 05975414db260e710e7b0129bd1960fcde1d8a51
</commit_message>
<xml_diff>
--- a/298-Ajout-de-l'évènement/ig/StructureDefinition-tddui-task-transport-professionnel.xlsx
+++ b/298-Ajout-de-l'évènement/ig/StructureDefinition-tddui-task-transport-professionnel.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3853" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3853" uniqueCount="525">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-17T15:38:22+00:00</t>
+    <t>2025-09-18T09:40:01+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -942,6 +942,9 @@
   </si>
   <si>
     <t>Period.end</t>
+  </si>
+  <si>
+    <t>dateFinTransport</t>
   </si>
   <si>
     <t>./high</t>
@@ -5642,31 +5645,31 @@
         <v>101</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
@@ -5688,14 +5691,14 @@
         <v>285</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>78</v>
@@ -5744,7 +5747,7 @@
         <v>78</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>79</v>
@@ -5753,7 +5756,7 @@
         <v>89</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>101</v>
@@ -5762,13 +5765,13 @@
         <v>78</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AO32" t="s" s="2">
         <v>78</v>
@@ -5776,14 +5779,14 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s" s="2">
@@ -5805,14 +5808,14 @@
         <v>285</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="P33" t="s" s="2">
         <v>78</v>
@@ -5861,7 +5864,7 @@
         <v>78</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>79</v>
@@ -5870,7 +5873,7 @@
         <v>89</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>101</v>
@@ -5882,7 +5885,7 @@
         <v>78</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>78</v>
@@ -5893,10 +5896,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5919,17 +5922,17 @@
         <v>90</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>78</v>
@@ -5978,7 +5981,7 @@
         <v>78</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>79</v>
@@ -5996,13 +5999,13 @@
         <v>78</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AO34" t="s" s="2">
         <v>78</v>
@@ -6010,10 +6013,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -6039,14 +6042,14 @@
         <v>195</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="P35" t="s" s="2">
         <v>78</v>
@@ -6074,10 +6077,10 @@
         <v>113</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="Z35" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AA35" t="s" s="2">
         <v>78</v>
@@ -6095,7 +6098,7 @@
         <v>78</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>79</v>
@@ -6113,13 +6116,13 @@
         <v>78</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>78</v>
@@ -6127,14 +6130,14 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
@@ -6153,19 +6156,19 @@
         <v>90</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="O36" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>78</v>
@@ -6214,7 +6217,7 @@
         <v>78</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>79</v>
@@ -6229,16 +6232,16 @@
         <v>101</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>78</v>
@@ -6246,10 +6249,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6272,17 +6275,17 @@
         <v>90</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>78</v>
@@ -6331,7 +6334,7 @@
         <v>78</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>79</v>
@@ -6349,13 +6352,13 @@
         <v>78</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>78</v>
@@ -6363,10 +6366,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6392,13 +6395,13 @@
         <v>195</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
@@ -6427,7 +6430,7 @@
         <v>199</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>78</v>
@@ -6448,7 +6451,7 @@
         <v>78</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>79</v>
@@ -6466,24 +6469,24 @@
         <v>78</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6509,13 +6512,13 @@
         <v>166</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
@@ -6565,7 +6568,7 @@
         <v>78</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>79</v>
@@ -6583,13 +6586,13 @@
         <v>78</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>78</v>
@@ -6597,10 +6600,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6623,13 +6626,13 @@
         <v>78</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6680,7 +6683,7 @@
         <v>78</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>79</v>
@@ -6698,24 +6701,24 @@
         <v>78</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AO40" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6738,13 +6741,13 @@
         <v>78</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -6795,7 +6798,7 @@
         <v>78</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>79</v>
@@ -6813,10 +6816,10 @@
         <v>78</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>78</v>
@@ -6827,14 +6830,14 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
@@ -6853,16 +6856,16 @@
         <v>78</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -6912,7 +6915,7 @@
         <v>78</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>79</v>
@@ -6930,10 +6933,10 @@
         <v>78</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>78</v>
@@ -6944,10 +6947,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6970,17 +6973,17 @@
         <v>78</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>78</v>
@@ -7029,7 +7032,7 @@
         <v>78</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>79</v>
@@ -7050,7 +7053,7 @@
         <v>78</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>78</v>
@@ -7061,10 +7064,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7176,10 +7179,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7293,14 +7296,14 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
@@ -7322,10 +7325,10 @@
         <v>135</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N46" t="s" s="2">
         <v>138</v>
@@ -7380,7 +7383,7 @@
         <v>78</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>79</v>
@@ -7412,10 +7415,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7438,17 +7441,17 @@
         <v>78</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="P47" t="s" s="2">
         <v>78</v>
@@ -7497,7 +7500,7 @@
         <v>78</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>79</v>
@@ -7518,7 +7521,7 @@
         <v>78</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>78</v>
@@ -7529,10 +7532,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7558,16 +7561,16 @@
         <v>267</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="O48" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>78</v>
@@ -7616,7 +7619,7 @@
         <v>78</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>79</v>
@@ -7637,7 +7640,7 @@
         <v>78</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>78</v>
@@ -7648,10 +7651,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7674,13 +7677,13 @@
         <v>78</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -7731,7 +7734,7 @@
         <v>78</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>79</v>
@@ -7752,7 +7755,7 @@
         <v>78</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>78</v>
@@ -7763,14 +7766,14 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
@@ -7789,17 +7792,17 @@
         <v>78</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>78</v>
@@ -7836,7 +7839,7 @@
         <v>78</v>
       </c>
       <c r="AB50" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AC50" s="2"/>
       <c r="AD50" t="s" s="2">
@@ -7846,7 +7849,7 @@
         <v>282</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>79</v>
@@ -7867,7 +7870,7 @@
         <v>78</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>78</v>
@@ -7878,10 +7881,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7993,10 +7996,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -8110,14 +8113,14 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" t="s" s="2">
@@ -8139,10 +8142,10 @@
         <v>135</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N53" t="s" s="2">
         <v>138</v>
@@ -8197,7 +8200,7 @@
         <v>78</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>79</v>
@@ -8229,14 +8232,14 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" t="s" s="2">
@@ -8258,16 +8261,16 @@
         <v>195</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="O54" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="P54" t="s" s="2">
         <v>78</v>
@@ -8295,7 +8298,7 @@
         <v>199</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>78</v>
@@ -8316,7 +8319,7 @@
         <v>78</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>89</v>
@@ -8337,7 +8340,7 @@
         <v>78</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>78</v>
@@ -8348,10 +8351,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8374,13 +8377,13 @@
         <v>78</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -8431,7 +8434,7 @@
         <v>78</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>89</v>
@@ -8452,7 +8455,7 @@
         <v>78</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>78</v>
@@ -8463,16 +8466,16 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C56" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D56" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
@@ -8491,17 +8494,17 @@
         <v>78</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P56" t="s" s="2">
         <v>78</v>
@@ -8550,7 +8553,7 @@
         <v>78</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>79</v>
@@ -8565,13 +8568,13 @@
         <v>101</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>78</v>
@@ -8582,10 +8585,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8697,10 +8700,10 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8814,14 +8817,14 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" t="s" s="2">
@@ -8843,10 +8846,10 @@
         <v>135</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N59" t="s" s="2">
         <v>138</v>
@@ -8901,7 +8904,7 @@
         <v>78</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>79</v>
@@ -8933,14 +8936,14 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" t="s" s="2">
@@ -8962,16 +8965,16 @@
         <v>195</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="O60" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="P60" t="s" s="2">
         <v>78</v>
@@ -8981,7 +8984,7 @@
         <v>78</v>
       </c>
       <c r="S60" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="T60" t="s" s="2">
         <v>78</v>
@@ -8999,7 +9002,7 @@
         <v>199</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>78</v>
@@ -9020,7 +9023,7 @@
         <v>78</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>89</v>
@@ -9041,7 +9044,7 @@
         <v>78</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>78</v>
@@ -9052,10 +9055,10 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -9081,10 +9084,10 @@
         <v>195</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -9115,7 +9118,7 @@
       </c>
       <c r="Y61" s="2"/>
       <c r="Z61" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AA61" t="s" s="2">
         <v>78</v>
@@ -9133,7 +9136,7 @@
         <v>78</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>89</v>
@@ -9154,7 +9157,7 @@
         <v>78</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>78</v>
@@ -9165,16 +9168,16 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C62" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D62" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" t="s" s="2">
@@ -9193,17 +9196,17 @@
         <v>78</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P62" t="s" s="2">
         <v>78</v>
@@ -9252,7 +9255,7 @@
         <v>78</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>79</v>
@@ -9267,13 +9270,13 @@
         <v>101</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>78</v>
@@ -9284,10 +9287,10 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9399,10 +9402,10 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9516,14 +9519,14 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" t="s" s="2">
@@ -9545,10 +9548,10 @@
         <v>135</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N65" t="s" s="2">
         <v>138</v>
@@ -9603,7 +9606,7 @@
         <v>78</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>79</v>
@@ -9635,14 +9638,14 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" t="s" s="2">
@@ -9664,16 +9667,16 @@
         <v>195</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="O66" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="P66" t="s" s="2">
         <v>78</v>
@@ -9683,7 +9686,7 @@
         <v>78</v>
       </c>
       <c r="S66" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="T66" t="s" s="2">
         <v>78</v>
@@ -9701,7 +9704,7 @@
         <v>199</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="Z66" t="s" s="2">
         <v>78</v>
@@ -9722,7 +9725,7 @@
         <v>78</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>89</v>
@@ -9743,7 +9746,7 @@
         <v>78</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN66" t="s" s="2">
         <v>78</v>
@@ -9754,10 +9757,10 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -9780,13 +9783,13 @@
         <v>78</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
@@ -9837,7 +9840,7 @@
         <v>78</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>89</v>
@@ -9858,7 +9861,7 @@
         <v>78</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN67" t="s" s="2">
         <v>78</v>
@@ -9869,16 +9872,16 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C68" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D68" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" t="s" s="2">
@@ -9897,17 +9900,17 @@
         <v>78</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P68" t="s" s="2">
         <v>78</v>
@@ -9956,7 +9959,7 @@
         <v>78</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>79</v>
@@ -9971,13 +9974,13 @@
         <v>101</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN68" t="s" s="2">
         <v>78</v>
@@ -9988,10 +9991,10 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -10103,10 +10106,10 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -10220,14 +10223,14 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" t="s" s="2">
@@ -10249,10 +10252,10 @@
         <v>135</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N71" t="s" s="2">
         <v>138</v>
@@ -10307,7 +10310,7 @@
         <v>78</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>79</v>
@@ -10339,14 +10342,14 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" t="s" s="2">
@@ -10368,16 +10371,16 @@
         <v>195</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N72" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="O72" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="P72" t="s" s="2">
         <v>78</v>
@@ -10387,7 +10390,7 @@
         <v>78</v>
       </c>
       <c r="S72" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="T72" t="s" s="2">
         <v>78</v>
@@ -10405,7 +10408,7 @@
         <v>199</v>
       </c>
       <c r="Y72" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="Z72" t="s" s="2">
         <v>78</v>
@@ -10426,7 +10429,7 @@
         <v>78</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>89</v>
@@ -10447,7 +10450,7 @@
         <v>78</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN72" t="s" s="2">
         <v>78</v>
@@ -10458,10 +10461,10 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10484,13 +10487,13 @@
         <v>78</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
@@ -10541,7 +10544,7 @@
         <v>78</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>89</v>
@@ -10562,7 +10565,7 @@
         <v>78</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN73" t="s" s="2">
         <v>78</v>
@@ -10573,16 +10576,16 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C74" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D74" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" t="s" s="2">
@@ -10601,17 +10604,17 @@
         <v>78</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P74" t="s" s="2">
         <v>78</v>
@@ -10660,7 +10663,7 @@
         <v>78</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>79</v>
@@ -10675,13 +10678,13 @@
         <v>101</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AL74" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN74" t="s" s="2">
         <v>78</v>
@@ -10692,10 +10695,10 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -10807,10 +10810,10 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
@@ -10924,14 +10927,14 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" t="s" s="2">
@@ -10953,10 +10956,10 @@
         <v>135</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N77" t="s" s="2">
         <v>138</v>
@@ -11011,7 +11014,7 @@
         <v>78</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>79</v>
@@ -11043,14 +11046,14 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" t="s" s="2">
@@ -11072,16 +11075,16 @@
         <v>195</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N78" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="O78" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="P78" t="s" s="2">
         <v>78</v>
@@ -11091,7 +11094,7 @@
         <v>78</v>
       </c>
       <c r="S78" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="T78" t="s" s="2">
         <v>78</v>
@@ -11109,7 +11112,7 @@
         <v>199</v>
       </c>
       <c r="Y78" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="Z78" t="s" s="2">
         <v>78</v>
@@ -11130,7 +11133,7 @@
         <v>78</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>89</v>
@@ -11151,7 +11154,7 @@
         <v>78</v>
       </c>
       <c r="AM78" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN78" t="s" s="2">
         <v>78</v>
@@ -11162,10 +11165,10 @@
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -11188,13 +11191,13 @@
         <v>78</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
@@ -11245,7 +11248,7 @@
         <v>78</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>89</v>
@@ -11266,7 +11269,7 @@
         <v>78</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN79" t="s" s="2">
         <v>78</v>
@@ -11277,16 +11280,16 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C80" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D80" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" t="s" s="2">
@@ -11305,17 +11308,17 @@
         <v>78</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P80" t="s" s="2">
         <v>78</v>
@@ -11364,7 +11367,7 @@
         <v>78</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AG80" t="s" s="2">
         <v>79</v>
@@ -11379,13 +11382,13 @@
         <v>101</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="AL80" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM80" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN80" t="s" s="2">
         <v>78</v>
@@ -11396,10 +11399,10 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -11511,10 +11514,10 @@
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
@@ -11628,14 +11631,14 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" t="s" s="2">
@@ -11657,10 +11660,10 @@
         <v>135</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N83" t="s" s="2">
         <v>138</v>
@@ -11715,7 +11718,7 @@
         <v>78</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG83" t="s" s="2">
         <v>79</v>
@@ -11747,14 +11750,14 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" t="s" s="2">
@@ -11776,16 +11779,16 @@
         <v>195</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="O84" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="P84" t="s" s="2">
         <v>78</v>
@@ -11795,7 +11798,7 @@
         <v>78</v>
       </c>
       <c r="S84" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="T84" t="s" s="2">
         <v>78</v>
@@ -11813,7 +11816,7 @@
         <v>199</v>
       </c>
       <c r="Y84" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="Z84" t="s" s="2">
         <v>78</v>
@@ -11834,7 +11837,7 @@
         <v>78</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>89</v>
@@ -11855,7 +11858,7 @@
         <v>78</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN84" t="s" s="2">
         <v>78</v>
@@ -11866,10 +11869,10 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
@@ -11892,13 +11895,13 @@
         <v>78</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="N85" s="2"/>
       <c r="O85" s="2"/>
@@ -11949,7 +11952,7 @@
         <v>78</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AG85" t="s" s="2">
         <v>89</v>
@@ -11970,7 +11973,7 @@
         <v>78</v>
       </c>
       <c r="AM85" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN85" t="s" s="2">
         <v>78</v>
@@ -11981,16 +11984,16 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C86" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D86" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" t="s" s="2">
@@ -12009,17 +12012,17 @@
         <v>78</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N86" s="2"/>
       <c r="O86" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P86" t="s" s="2">
         <v>78</v>
@@ -12068,7 +12071,7 @@
         <v>78</v>
       </c>
       <c r="AF86" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AG86" t="s" s="2">
         <v>79</v>
@@ -12083,13 +12086,13 @@
         <v>101</v>
       </c>
       <c r="AK86" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="AL86" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM86" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN86" t="s" s="2">
         <v>78</v>
@@ -12100,10 +12103,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
@@ -12215,10 +12218,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
@@ -12332,14 +12335,14 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" t="s" s="2">
@@ -12361,10 +12364,10 @@
         <v>135</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N89" t="s" s="2">
         <v>138</v>
@@ -12419,7 +12422,7 @@
         <v>78</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG89" t="s" s="2">
         <v>79</v>
@@ -12451,14 +12454,14 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" t="s" s="2">
@@ -12480,16 +12483,16 @@
         <v>195</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N90" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="O90" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="P90" t="s" s="2">
         <v>78</v>
@@ -12499,7 +12502,7 @@
         <v>78</v>
       </c>
       <c r="S90" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="T90" t="s" s="2">
         <v>78</v>
@@ -12517,7 +12520,7 @@
         <v>199</v>
       </c>
       <c r="Y90" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="Z90" t="s" s="2">
         <v>78</v>
@@ -12538,7 +12541,7 @@
         <v>78</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>89</v>
@@ -12559,7 +12562,7 @@
         <v>78</v>
       </c>
       <c r="AM90" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN90" t="s" s="2">
         <v>78</v>
@@ -12570,10 +12573,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
@@ -12596,13 +12599,13 @@
         <v>78</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="M91" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
@@ -12653,7 +12656,7 @@
         <v>78</v>
       </c>
       <c r="AF91" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AG91" t="s" s="2">
         <v>89</v>
@@ -12674,7 +12677,7 @@
         <v>78</v>
       </c>
       <c r="AM91" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN91" t="s" s="2">
         <v>78</v>
@@ -12685,16 +12688,16 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C92" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D92" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" t="s" s="2">
@@ -12713,17 +12716,17 @@
         <v>78</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="M92" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N92" s="2"/>
       <c r="O92" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P92" t="s" s="2">
         <v>78</v>
@@ -12772,7 +12775,7 @@
         <v>78</v>
       </c>
       <c r="AF92" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AG92" t="s" s="2">
         <v>79</v>
@@ -12787,13 +12790,13 @@
         <v>101</v>
       </c>
       <c r="AK92" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="AL92" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM92" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN92" t="s" s="2">
         <v>78</v>
@@ -12804,10 +12807,10 @@
     </row>
     <row r="93">
       <c r="A93" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" t="s" s="2">
@@ -12919,10 +12922,10 @@
     </row>
     <row r="94">
       <c r="A94" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B94" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" t="s" s="2">
@@ -13036,14 +13039,14 @@
     </row>
     <row r="95">
       <c r="A95" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B95" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" t="s" s="2">
@@ -13065,10 +13068,10 @@
         <v>135</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M95" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N95" t="s" s="2">
         <v>138</v>
@@ -13123,7 +13126,7 @@
         <v>78</v>
       </c>
       <c r="AF95" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG95" t="s" s="2">
         <v>79</v>
@@ -13155,14 +13158,14 @@
     </row>
     <row r="96">
       <c r="A96" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B96" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" t="s" s="2">
@@ -13184,16 +13187,16 @@
         <v>195</v>
       </c>
       <c r="L96" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M96" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N96" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="O96" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="P96" t="s" s="2">
         <v>78</v>
@@ -13203,7 +13206,7 @@
         <v>78</v>
       </c>
       <c r="S96" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="T96" t="s" s="2">
         <v>78</v>
@@ -13221,7 +13224,7 @@
         <v>199</v>
       </c>
       <c r="Y96" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="Z96" t="s" s="2">
         <v>78</v>
@@ -13242,7 +13245,7 @@
         <v>78</v>
       </c>
       <c r="AF96" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AG96" t="s" s="2">
         <v>89</v>
@@ -13263,7 +13266,7 @@
         <v>78</v>
       </c>
       <c r="AM96" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN96" t="s" s="2">
         <v>78</v>
@@ -13274,10 +13277,10 @@
     </row>
     <row r="97">
       <c r="A97" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B97" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" t="s" s="2">
@@ -13300,13 +13303,13 @@
         <v>78</v>
       </c>
       <c r="K97" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="L97" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="M97" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
@@ -13357,7 +13360,7 @@
         <v>78</v>
       </c>
       <c r="AF97" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AG97" t="s" s="2">
         <v>89</v>
@@ -13378,7 +13381,7 @@
         <v>78</v>
       </c>
       <c r="AM97" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN97" t="s" s="2">
         <v>78</v>
@@ -13389,10 +13392,10 @@
     </row>
     <row r="98">
       <c r="A98" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B98" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" t="s" s="2">
@@ -13415,17 +13418,17 @@
         <v>78</v>
       </c>
       <c r="K98" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="L98" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="M98" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="N98" s="2"/>
       <c r="O98" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="P98" t="s" s="2">
         <v>78</v>
@@ -13474,7 +13477,7 @@
         <v>78</v>
       </c>
       <c r="AF98" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="AG98" t="s" s="2">
         <v>79</v>
@@ -13495,7 +13498,7 @@
         <v>78</v>
       </c>
       <c r="AM98" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN98" t="s" s="2">
         <v>78</v>
@@ -13506,10 +13509,10 @@
     </row>
     <row r="99">
       <c r="A99" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B99" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" t="s" s="2">
@@ -13621,10 +13624,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B100" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" t="s" s="2">
@@ -13738,14 +13741,14 @@
     </row>
     <row r="101">
       <c r="A101" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B101" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" t="s" s="2">
@@ -13767,10 +13770,10 @@
         <v>135</v>
       </c>
       <c r="L101" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M101" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N101" t="s" s="2">
         <v>138</v>
@@ -13825,7 +13828,7 @@
         <v>78</v>
       </c>
       <c r="AF101" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG101" t="s" s="2">
         <v>79</v>
@@ -13857,14 +13860,14 @@
     </row>
     <row r="102">
       <c r="A102" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B102" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" t="s" s="2">
@@ -13886,14 +13889,14 @@
         <v>195</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="M102" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="N102" s="2"/>
       <c r="O102" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="P102" t="s" s="2">
         <v>78</v>
@@ -13921,7 +13924,7 @@
         <v>199</v>
       </c>
       <c r="Y102" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="Z102" t="s" s="2">
         <v>78</v>
@@ -13942,7 +13945,7 @@
         <v>78</v>
       </c>
       <c r="AF102" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="AG102" t="s" s="2">
         <v>89</v>
@@ -13963,7 +13966,7 @@
         <v>78</v>
       </c>
       <c r="AM102" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN102" t="s" s="2">
         <v>78</v>
@@ -13974,10 +13977,10 @@
     </row>
     <row r="103">
       <c r="A103" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B103" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" t="s" s="2">
@@ -14000,17 +14003,17 @@
         <v>78</v>
       </c>
       <c r="K103" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="L103" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="M103" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="N103" s="2"/>
       <c r="O103" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="P103" t="s" s="2">
         <v>78</v>
@@ -14059,7 +14062,7 @@
         <v>78</v>
       </c>
       <c r="AF103" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="AG103" t="s" s="2">
         <v>89</v>
@@ -14080,7 +14083,7 @@
         <v>78</v>
       </c>
       <c r="AM103" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN103" t="s" s="2">
         <v>78</v>

</xml_diff>

<commit_message>
Update suite aux retours sur la PR a4cb814016031e652382c1507ba6cc56898e3c0a
</commit_message>
<xml_diff>
--- a/298-Ajout-de-l'évènement/ig/StructureDefinition-tddui-task-transport-professionnel.xlsx
+++ b/298-Ajout-de-l'évènement/ig/StructureDefinition-tddui-task-transport-professionnel.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3853" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3853" uniqueCount="523">
   <si>
     <t>Property</t>
   </si>
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Transport Professionnel</t>
+    <t>TDDUI Task Transport Professionnel</t>
   </si>
   <si>
     <t>Status</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-18T14:47:30+00:00</t>
+    <t>2025-09-23T09:18:22+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1561,9 +1561,6 @@
     <t>Distance du trajet</t>
   </si>
   <si>
-    <t>distanceTrajet</t>
-  </si>
-  <si>
     <t>Task.input:distance.id</t>
   </si>
   <si>
@@ -1598,9 +1595,6 @@
   </si>
   <si>
     <t>Durée théorique du trajet</t>
-  </si>
-  <si>
-    <t>dureeTheoriqueTrajet</t>
   </si>
   <si>
     <t>Task.input:dureeTheorique.id</t>
@@ -12086,7 +12080,7 @@
         <v>101</v>
       </c>
       <c r="AK86" t="s" s="2">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="AL86" t="s" s="2">
         <v>78</v>
@@ -12103,7 +12097,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B87" t="s" s="2">
         <v>425</v>
@@ -12218,7 +12212,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B88" t="s" s="2">
         <v>426</v>
@@ -12335,7 +12329,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B89" t="s" s="2">
         <v>427</v>
@@ -12454,7 +12448,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B90" t="s" s="2">
         <v>428</v>
@@ -12502,7 +12496,7 @@
         <v>78</v>
       </c>
       <c r="S90" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T90" t="s" s="2">
         <v>78</v>
@@ -12573,7 +12567,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B91" t="s" s="2">
         <v>435</v>
@@ -12599,7 +12593,7 @@
         <v>78</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L91" t="s" s="2">
         <v>437</v>
@@ -12688,13 +12682,13 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="2">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B92" t="s" s="2">
         <v>418</v>
       </c>
       <c r="C92" t="s" s="2">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D92" t="s" s="2">
         <v>419</v>
@@ -12719,7 +12713,7 @@
         <v>389</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="M92" t="s" s="2">
         <v>421</v>
@@ -12790,7 +12784,7 @@
         <v>101</v>
       </c>
       <c r="AK92" t="s" s="2">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="AL92" t="s" s="2">
         <v>78</v>
@@ -12807,7 +12801,7 @@
     </row>
     <row r="93">
       <c r="A93" t="s" s="2">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B93" t="s" s="2">
         <v>425</v>
@@ -12922,7 +12916,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s" s="2">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B94" t="s" s="2">
         <v>426</v>
@@ -13039,7 +13033,7 @@
     </row>
     <row r="95">
       <c r="A95" t="s" s="2">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B95" t="s" s="2">
         <v>427</v>
@@ -13158,7 +13152,7 @@
     </row>
     <row r="96">
       <c r="A96" t="s" s="2">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B96" t="s" s="2">
         <v>428</v>
@@ -13206,7 +13200,7 @@
         <v>78</v>
       </c>
       <c r="S96" t="s" s="2">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="T96" t="s" s="2">
         <v>78</v>
@@ -13277,7 +13271,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s" s="2">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B97" t="s" s="2">
         <v>435</v>
@@ -13303,7 +13297,7 @@
         <v>78</v>
       </c>
       <c r="K97" t="s" s="2">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="L97" t="s" s="2">
         <v>437</v>
@@ -13392,10 +13386,10 @@
     </row>
     <row r="98">
       <c r="A98" t="s" s="2">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B98" t="s" s="2">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" t="s" s="2">
@@ -13421,14 +13415,14 @@
         <v>389</v>
       </c>
       <c r="L98" t="s" s="2">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="M98" t="s" s="2">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N98" s="2"/>
       <c r="O98" t="s" s="2">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="P98" t="s" s="2">
         <v>78</v>
@@ -13477,7 +13471,7 @@
         <v>78</v>
       </c>
       <c r="AF98" t="s" s="2">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="AG98" t="s" s="2">
         <v>79</v>
@@ -13509,10 +13503,10 @@
     </row>
     <row r="99">
       <c r="A99" t="s" s="2">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B99" t="s" s="2">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" t="s" s="2">
@@ -13624,10 +13618,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s" s="2">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B100" t="s" s="2">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" t="s" s="2">
@@ -13741,10 +13735,10 @@
     </row>
     <row r="101">
       <c r="A101" t="s" s="2">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B101" t="s" s="2">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" t="s" s="2">
@@ -13860,10 +13854,10 @@
     </row>
     <row r="102">
       <c r="A102" t="s" s="2">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B102" t="s" s="2">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" t="s" s="2">
@@ -13889,14 +13883,14 @@
         <v>195</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="M102" t="s" s="2">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="N102" s="2"/>
       <c r="O102" t="s" s="2">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="P102" t="s" s="2">
         <v>78</v>
@@ -13924,7 +13918,7 @@
         <v>199</v>
       </c>
       <c r="Y102" t="s" s="2">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="Z102" t="s" s="2">
         <v>78</v>
@@ -13945,7 +13939,7 @@
         <v>78</v>
       </c>
       <c r="AF102" t="s" s="2">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="AG102" t="s" s="2">
         <v>89</v>
@@ -13977,10 +13971,10 @@
     </row>
     <row r="103">
       <c r="A103" t="s" s="2">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B103" t="s" s="2">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" t="s" s="2">
@@ -14006,14 +14000,14 @@
         <v>436</v>
       </c>
       <c r="L103" t="s" s="2">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="M103" t="s" s="2">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="N103" s="2"/>
       <c r="O103" t="s" s="2">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="P103" t="s" s="2">
         <v>78</v>
@@ -14062,7 +14056,7 @@
         <v>78</v>
       </c>
       <c r="AF103" t="s" s="2">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="AG103" t="s" s="2">
         <v>89</v>

</xml_diff>